<commit_message>
fixed : tag level on tab tag page dataset, added : dataset delivery_format
</commit_message>
<xml_diff>
--- a/public/data/db_source/__metaVariable__.xlsx
+++ b/public/data/db_source/__metaVariable__.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannuaire/datannuaire_dev/db/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464874B9-BA8E-AE40-BDE6-F7D77C73398B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EC92E5-5E75-1E4D-9332-BD2D86CDFAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2680" yWindow="500" windowWidth="26120" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="164">
   <si>
     <t>id</t>
   </si>
@@ -525,6 +525,9 @@
   </si>
   <si>
     <t>emplacement des métadonnées du dossier</t>
+  </si>
+  <si>
+    <t>Format du dataset livrées (CSV, XML, ...)</t>
   </si>
 </sst>
 </file>
@@ -580,10 +583,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}" name="Tableau3" displayName="Tableau3" ref="A1:C110" totalsRowShown="0">
-  <autoFilter ref="A1:C110" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C110">
-    <sortCondition ref="B1:B110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}" name="Tableau3" displayName="Tableau3" ref="A1:C111" totalsRowShown="0">
+  <autoFilter ref="A1:C111" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C111">
+    <sortCondition ref="B1:B111"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C890023E-DEFC-5144-9523-0CAD4553F8F1}" name="variable"/>
@@ -916,11 +919,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C110"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,1002 +1144,1013 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="B23" t="s">
-        <v>119</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="B24" t="s">
         <v>119</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="B25" t="s">
         <v>119</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>119</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
         <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
         <v>119</v>
       </c>
       <c r="C28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
         <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
         <v>119</v>
       </c>
       <c r="C30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="B32" t="s">
         <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
         <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B35" t="s">
         <v>124</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C36" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="B37" t="s">
         <v>127</v>
       </c>
       <c r="C37" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
         <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
         <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
         <v>28</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
         <v>28</v>
       </c>
       <c r="C43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B44" t="s">
         <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
         <v>28</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B46" t="s">
         <v>28</v>
       </c>
       <c r="C46" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
         <v>28</v>
       </c>
       <c r="C47" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B48" t="s">
         <v>28</v>
       </c>
       <c r="C48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="B49" t="s">
         <v>28</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="B50" t="s">
         <v>28</v>
       </c>
       <c r="C50" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B51" t="s">
         <v>28</v>
       </c>
       <c r="C51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="B52" t="s">
         <v>28</v>
       </c>
       <c r="C52" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
         <v>28</v>
       </c>
       <c r="C53" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B54" t="s">
         <v>28</v>
       </c>
       <c r="C54" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="B55" t="s">
-        <v>125</v>
+        <v>28</v>
       </c>
       <c r="C55" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B56" t="s">
         <v>125</v>
       </c>
       <c r="C56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="C57" t="s">
-        <v>56</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B58" t="s">
         <v>104</v>
       </c>
       <c r="C58" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B59" t="s">
         <v>104</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B60" t="s">
         <v>104</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B61" t="s">
         <v>104</v>
       </c>
       <c r="C61" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="B62" t="s">
         <v>104</v>
       </c>
       <c r="C62" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B63" t="s">
         <v>104</v>
       </c>
       <c r="C63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C64" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="B65" t="s">
         <v>95</v>
       </c>
       <c r="C65" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
         <v>95</v>
       </c>
       <c r="C66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B67" t="s">
         <v>95</v>
       </c>
       <c r="C67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B68" t="s">
         <v>95</v>
       </c>
       <c r="C68" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="B69" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="C69" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="B70" t="s">
         <v>30</v>
       </c>
       <c r="C70" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="B71" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="C71" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B72" t="s">
         <v>79</v>
       </c>
       <c r="C72" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B73" t="s">
         <v>79</v>
       </c>
       <c r="C73" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B74" t="s">
         <v>79</v>
       </c>
       <c r="C74" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B75" t="s">
         <v>79</v>
       </c>
       <c r="C75" t="s">
-        <v>126</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B76" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C76" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B77" t="s">
         <v>87</v>
       </c>
       <c r="C77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="C78" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="B79" t="s">
         <v>29</v>
       </c>
       <c r="C79" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="B80" t="s">
-        <v>129</v>
+        <v>29</v>
       </c>
       <c r="C80" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="B81" t="s">
         <v>129</v>
       </c>
       <c r="C81" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B82" t="s">
         <v>129</v>
       </c>
       <c r="C82" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="B83" t="s">
         <v>129</v>
       </c>
       <c r="C83" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="B84" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="C84" t="s">
-        <v>60</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B85" t="s">
         <v>21</v>
       </c>
       <c r="C85" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B86" t="s">
         <v>21</v>
       </c>
       <c r="C86" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B87" t="s">
-        <v>121</v>
+        <v>21</v>
       </c>
       <c r="C87" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B88" t="s">
         <v>121</v>
       </c>
       <c r="C88" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B89" t="s">
         <v>121</v>
       </c>
       <c r="C89" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B90" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C90" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B91" t="s">
         <v>122</v>
       </c>
       <c r="C91" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B92" t="s">
         <v>122</v>
       </c>
       <c r="C92" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B93" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C93" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="B94" t="s">
         <v>123</v>
       </c>
       <c r="C94" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="B95" t="s">
         <v>123</v>
       </c>
       <c r="C95" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B96" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="C96" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="B97" t="s">
         <v>22</v>
       </c>
       <c r="C97" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="B98" t="s">
         <v>22</v>
       </c>
       <c r="C98" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B99" t="s">
         <v>22</v>
       </c>
       <c r="C99" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B100" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C100" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B101" t="s">
         <v>23</v>
       </c>
       <c r="C101" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B102" t="s">
         <v>23</v>
       </c>
       <c r="C102" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B103" t="s">
         <v>23</v>
       </c>
       <c r="C103" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B104" t="s">
         <v>23</v>
       </c>
       <c r="C104" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B105" t="s">
         <v>23</v>
       </c>
       <c r="C105" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B106" t="s">
         <v>23</v>
       </c>
       <c r="C106" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B107" t="s">
         <v>23</v>
       </c>
       <c r="C107" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B108" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="C108" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B109" t="s">
         <v>78</v>
       </c>
       <c r="C109" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="B110" t="s">
         <v>78</v>
       </c>
       <c r="C110" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>84</v>
+      </c>
+      <c r="B111" t="s">
+        <v>78</v>
+      </c>
+      <c r="C111" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>